<commit_message>
lrfr positive flexure almost sorted out
</commit_message>
<xml_diff>
--- a/data/sectionprops.xlsx
+++ b/data/sectionprops.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
   <si>
     <t>Span Length</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>Es</t>
+  </si>
+  <si>
+    <t>Number of spans</t>
+  </si>
+  <si>
+    <t>nSpans</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>desc</t>
   </si>
 </sst>
 </file>
@@ -518,15 +530,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,251 +547,265 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>1428</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="D3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>324</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>29000000</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
       </c>
-      <c r="D5">
-        <v>4</v>
+      <c r="D5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>36000</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
       </c>
-      <c r="D6">
-        <v>5</v>
+      <c r="D6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>4000</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>8.5</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="D8">
-        <v>7</v>
+      <c r="D8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>92</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9">
-        <v>8</v>
+      <c r="D9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="D10">
-        <v>9</v>
+      <c r="D10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D11">
-        <v>10</v>
+      <c r="D11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>0.5625</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="D12">
-        <v>11</v>
+      <c r="D12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="D13">
-        <v>12</v>
+      <c r="D13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>0.75</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="D14">
-        <v>13</v>
+      <c r="D14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="D15">
-        <v>14</v>
+      <c r="D15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>1.5</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>109</v>
       </c>
       <c r="C17" t="s">
         <v>49</v>
       </c>
-      <c r="D17">
-        <v>16</v>
+      <c r="D17" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
       </c>
       <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="D18">
-        <v>17</v>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
general clean up. added examples directory
</commit_message>
<xml_diff>
--- a/data/sectionprops.xlsx
+++ b/data/sectionprops.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="105" windowWidth="21075" windowHeight="10545"/>
   </bookViews>
   <sheets>
-    <sheet name="LRFR" sheetId="1" r:id="rId1"/>
+    <sheet name="example1" sheetId="1" r:id="rId1"/>
     <sheet name="LFR" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -533,7 +533,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated readme w/ examples
</commit_message>
<xml_diff>
--- a/data/sectionprops.xlsx
+++ b/data/sectionprops.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
   <si>
     <t>Span Length</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>desc</t>
+  </si>
+  <si>
+    <t>panel</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Panel location of section [interior/end]</t>
   </si>
 </sst>
 </file>
@@ -530,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,239 +581,253 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3">
-        <v>1428</v>
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4">
-        <v>324</v>
+        <v>1428</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5">
-        <v>29000000</v>
+        <v>324</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B6">
-        <v>36000</v>
+        <v>29000000</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>4000</v>
+        <v>36000</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>8.5</v>
+        <v>4000</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>92</v>
+        <v>8.5</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12">
-        <v>0.5625</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13">
-        <v>14</v>
+        <v>0.5625</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>0.75</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>0.75</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
-        <v>1.5</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17">
-        <v>109</v>
+        <v>1.5</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
         <v>49</v>
       </c>
       <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>